<commit_message>
Version final del excel con los calculos
</commit_message>
<xml_diff>
--- a/resource/output.xlsx
+++ b/resource/output.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnco-my.sharepoint.com/personal/endo_rodriguez_externos-co_cencosud_com/Documents/Documentos/Scrip cuadratura/cuadratura/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_48ABCB7C1872680E6235547658E616BE91ECC9DA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F717833-C18D-4D47-B4A2-A05819C5849F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_273784695F5F600F62355476585DCE3A87CED18D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{959196A9-E49E-42A4-AD28-8F5CE8E4C63E}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2895" yWindow="2895" windowWidth="14745" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>cajero</t>
   </si>
@@ -67,22 +80,82 @@
     <t>Factura</t>
   </si>
   <si>
-    <t>00000020898908</t>
-  </si>
-  <si>
-    <t>00000020257514</t>
-  </si>
-  <si>
-    <t>00000020272784</t>
-  </si>
-  <si>
-    <t>00000041024355</t>
-  </si>
-  <si>
-    <t>00000077063342</t>
-  </si>
-  <si>
-    <t>00000020036133</t>
+    <t>00000002500139</t>
+  </si>
+  <si>
+    <t>00000078600010</t>
+  </si>
+  <si>
+    <t>07702044253420</t>
+  </si>
+  <si>
+    <t>00080432105528</t>
+  </si>
+  <si>
+    <t>00000002500281</t>
+  </si>
+  <si>
+    <t>07702132002671</t>
+  </si>
+  <si>
+    <t>07702085012093</t>
+  </si>
+  <si>
+    <t>07702425546226</t>
+  </si>
+  <si>
+    <t>07702001133611</t>
+  </si>
+  <si>
+    <t>07702450011119</t>
+  </si>
+  <si>
+    <t>00000002503714</t>
+  </si>
+  <si>
+    <t>00000020037567</t>
+  </si>
+  <si>
+    <t>00799366186311</t>
+  </si>
+  <si>
+    <t>07707275650505</t>
+  </si>
+  <si>
+    <t>07702714100054</t>
+  </si>
+  <si>
+    <t>07702084137520</t>
+  </si>
+  <si>
+    <t>07702085019023</t>
+  </si>
+  <si>
+    <t>07702024341338</t>
+  </si>
+  <si>
+    <t>07702136645058</t>
+  </si>
+  <si>
+    <t>07702057162399</t>
+  </si>
+  <si>
+    <t>00000002503708</t>
+  </si>
+  <si>
+    <t>00000002503715</t>
+  </si>
+  <si>
+    <t>00000002504016</t>
+  </si>
+  <si>
+    <t>00000002503264</t>
+  </si>
+  <si>
+    <t>00000002504014</t>
+  </si>
+  <si>
+    <t>00000002501235</t>
   </si>
 </sst>
 </file>
@@ -445,15 +518,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection sqref="A1:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -508,34 +582,43 @@
         <v>1116666729</v>
       </c>
       <c r="B2">
-        <v>2301</v>
+        <v>2340</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>4218</v>
+        <v>7333</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2">
-        <v>1261</v>
+        <v>5825</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>239</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>466</v>
+      </c>
+      <c r="K2">
+        <v>-26699</v>
       </c>
       <c r="L2">
-        <v>70641</v>
+        <v>-240291</v>
       </c>
       <c r="M2">
-        <v>-41</v>
+        <v>41</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -543,19 +626,13 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <v>34407</v>
+        <v>1626</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>2753</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -563,19 +640,13 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>12954</v>
+        <v>8766</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1036</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -583,19 +654,19 @@
         <v>18</v>
       </c>
       <c r="F5">
-        <v>9082</v>
+        <v>125276</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>1726</v>
+        <v>6264</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5">
-        <v>582</v>
+        <v>33151</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -603,19 +674,13 @@
         <v>19</v>
       </c>
       <c r="F6">
-        <v>2804</v>
+        <v>7065</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>533</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>3263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -623,13 +688,848 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>19431</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>2100</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>23571</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>4671</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1116666729</v>
+      </c>
+      <c r="B11">
+        <v>2340</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>7337</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>6472</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>518</v>
+      </c>
+      <c r="L11">
+        <v>-58720</v>
+      </c>
+      <c r="M11">
+        <v>-30</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>9739</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>1807</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>27839</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1392</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>8759</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1116666729</v>
+      </c>
+      <c r="B15">
+        <v>2340</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>7330</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15">
+        <v>4671</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>29321</v>
+      </c>
+      <c r="L15">
+        <v>263889</v>
+      </c>
+      <c r="M15">
+        <v>-39</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>5825</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17">
+        <v>1625</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>8766</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>1626</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20">
+        <v>2874</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>45000</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22">
+        <v>3591</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>5391</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>8554</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>5306</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26">
+        <v>3141</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27">
+        <v>3591</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28">
+        <v>18171</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29">
+        <v>6300</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30">
+        <v>15000</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31">
+        <v>29933</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32">
+        <v>33300</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33">
+        <v>29925</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>16975</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1116666729</v>
+      </c>
+      <c r="B35">
+        <v>2340</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>7338</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>4671</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>-29321</v>
+      </c>
+      <c r="L35">
+        <v>-263889</v>
+      </c>
+      <c r="M35">
+        <v>39</v>
+      </c>
+      <c r="O35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>5825</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37">
+        <v>1625</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38">
+        <v>8766</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39">
+        <v>1626</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40">
+        <v>2874</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41">
+        <v>45000</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42">
+        <v>3591</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43">
+        <v>5391</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44">
+        <v>8554</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45">
+        <v>5306</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46">
+        <v>3141</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47">
+        <v>3591</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48">
+        <v>18171</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49">
+        <v>6300</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50">
+        <v>15000</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51">
+        <v>29933</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52">
+        <v>33300</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F53">
+        <v>29925</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54">
+        <v>16975</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>